<commit_message>
[Nico] - Writing v0.6.1 - Latex Error Persists
</commit_message>
<xml_diff>
--- a/excels/writing.xlsx
+++ b/excels/writing.xlsx
@@ -218,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -280,6 +280,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,7 +371,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -543,7 +547,7 @@
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
-      <c r="D13" s="9"/>
+      <c r="D13" s="16"/>
       <c r="H13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -552,7 +556,7 @@
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="9"/>
+      <c r="D14" s="16"/>
       <c r="H14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,7 +595,7 @@
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
-      <c r="D18" s="16"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>

</xml_diff>

<commit_message>
[Nico] - Writing v1.0 - Updated before F. Feedback 1
</commit_message>
<xml_diff>
--- a/excels/writing.xlsx
+++ b/excels/writing.xlsx
@@ -267,6 +267,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -275,19 +279,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -371,7 +371,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -468,23 +468,26 @@
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
-      <c r="D5" s="9"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -499,7 +502,10 @@
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,23 +514,26 @@
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
-      <c r="D9" s="9"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
       <c r="H9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -538,7 +547,11 @@
         <v>14</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="D12" s="9"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,7 +560,10 @@
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
-      <c r="D13" s="16"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
       <c r="H13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,23 +572,26 @@
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="16"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -586,29 +605,38 @@
         <v>9</v>
       </c>
       <c r="B17" s="11"/>
-      <c r="D17" s="9"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
       <c r="H17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="9"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
       <c r="H19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -634,8 +662,12 @@
       <c r="C22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="H22" s="9"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>